<commit_message>
Update of Rab data
</commit_message>
<xml_diff>
--- a/data/variance/variance Rabs.xlsx
+++ b/data/variance/variance Rabs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u1455231/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/Documents/Manuscripts/In progress/CellMigration/Figures/RabMap/Rab Variance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B18F67-4126-1D4F-8109-FBC4A8B14CD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2FDD527-A091-7F49-B925-583D3C6F186B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14600" activeTab="3" xr2:uid="{864B79E4-4330-D74D-8368-11D16301E11D}"/>
   </bookViews>
@@ -16,7 +16,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="MeansForExport" sheetId="4" r:id="rId4"/>
+    <sheet name="Notes" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$B$1:$B$1575</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3584" uniqueCount="1615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3586" uniqueCount="1617">
   <si>
     <t>150120HeLa_GFP-Rab33b 4-1.tif</t>
   </si>
@@ -4876,6 +4877,12 @@
   </si>
   <si>
     <t>Rab43</t>
+  </si>
+  <si>
+    <t>GFP-Rab17 images are actually of GFP-Rab24</t>
+  </si>
+  <si>
+    <t>GFP-Rab24 images are actually of GFP-Rab17</t>
   </si>
 </sst>
 </file>
@@ -28510,7 +28517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{715CAFAC-4E66-824F-A3A3-BE5A0C74EEE8}">
   <dimension ref="A1:B394"/>
   <sheetViews>
-    <sheetView topLeftCell="A371" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B385" sqref="B385:B394"/>
     </sheetView>
   </sheetViews>
@@ -31680,8 +31687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9039DB9-EA86-6544-AE9F-764874238E8C}">
   <dimension ref="A1:AN11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L11"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -31867,7 +31874,7 @@
         <v>1.5762133000000001E-2</v>
       </c>
       <c r="T2">
-        <v>9.5888318750000003E-3</v>
+        <v>7.3516355999999998E-3</v>
       </c>
       <c r="U2">
         <v>1.0182360775E-2</v>
@@ -31888,7 +31895,7 @@
         <v>3.1001079500000001E-3</v>
       </c>
       <c r="AA2">
-        <v>7.3516355999999998E-3</v>
+        <v>9.5888318750000003E-3</v>
       </c>
       <c r="AB2">
         <v>9.8620273249999998E-3</v>
@@ -31989,7 +31996,7 @@
         <v>1.52151275E-2</v>
       </c>
       <c r="T3">
-        <v>5.5035640250000002E-3</v>
+        <v>1.4948858500000002E-2</v>
       </c>
       <c r="U3">
         <v>1.275477685E-2</v>
@@ -32010,7 +32017,7 @@
         <v>7.414689625E-3</v>
       </c>
       <c r="AA3">
-        <v>1.4948858500000002E-2</v>
+        <v>5.5035640250000002E-3</v>
       </c>
       <c r="AB3">
         <v>1.16099429E-2</v>
@@ -32111,7 +32118,7 @@
         <v>5.9340094500000004E-3</v>
       </c>
       <c r="T4">
-        <v>3.5484552499999997E-3</v>
+        <v>1.4840648E-2</v>
       </c>
       <c r="U4">
         <v>1.1551415225E-2</v>
@@ -32132,7 +32139,7 @@
         <v>2.2999301249999999E-3</v>
       </c>
       <c r="AA4">
-        <v>1.4840648E-2</v>
+        <v>3.5484552499999997E-3</v>
       </c>
       <c r="AB4">
         <v>1.8396835E-2</v>
@@ -32233,7 +32240,7 @@
         <v>1.453346225E-2</v>
       </c>
       <c r="T5">
-        <v>8.8452106749999995E-3</v>
+        <v>1.370834525E-2</v>
       </c>
       <c r="U5">
         <v>1.4094499325000003E-2</v>
@@ -32254,7 +32261,7 @@
         <v>4.0284438250000002E-3</v>
       </c>
       <c r="AA5">
-        <v>1.370834525E-2</v>
+        <v>8.8452106749999995E-3</v>
       </c>
       <c r="AB5">
         <v>2.313240875E-2</v>
@@ -32355,7 +32362,7 @@
         <v>1.313217475E-2</v>
       </c>
       <c r="T6">
-        <v>4.7303620499999999E-3</v>
+        <v>1.6840965999999999E-2</v>
       </c>
       <c r="U6">
         <v>9.8796578999999999E-3</v>
@@ -32376,7 +32383,7 @@
         <v>7.0211189999999993E-3</v>
       </c>
       <c r="AA6">
-        <v>1.6840965999999999E-2</v>
+        <v>4.7303620499999999E-3</v>
       </c>
       <c r="AB6">
         <v>1.2053775500000001E-2</v>
@@ -32477,7 +32484,7 @@
         <v>1.479001275E-2</v>
       </c>
       <c r="T7">
-        <v>4.0619127999999994E-3</v>
+        <v>1.1292105624999998E-2</v>
       </c>
       <c r="U7">
         <v>1.5137948424999999E-2</v>
@@ -32498,7 +32505,7 @@
         <v>3.8246914249999999E-3</v>
       </c>
       <c r="AA7">
-        <v>1.1292105624999998E-2</v>
+        <v>4.0619127999999994E-3</v>
       </c>
       <c r="AB7">
         <v>1.512676925E-2</v>
@@ -32599,7 +32606,7 @@
         <v>1.1043792049999999E-2</v>
       </c>
       <c r="T8">
-        <v>7.7699587750000004E-3</v>
+        <v>1.4406406500000002E-2</v>
       </c>
       <c r="U8">
         <v>1.687589125E-2</v>
@@ -32620,7 +32627,7 @@
         <v>3.2738502749999998E-3</v>
       </c>
       <c r="AA8">
-        <v>1.4406406500000002E-2</v>
+        <v>7.7699587750000004E-3</v>
       </c>
       <c r="AB8">
         <v>2.0340637624999998E-2</v>
@@ -32721,7 +32728,7 @@
         <v>8.42408945E-3</v>
       </c>
       <c r="T9">
-        <v>9.9139316999999998E-3</v>
+        <v>1.177409825E-2</v>
       </c>
       <c r="U9">
         <v>1.3544523675E-2</v>
@@ -32742,7 +32749,7 @@
         <v>3.1729522749999999E-3</v>
       </c>
       <c r="AA9">
-        <v>1.177409825E-2</v>
+        <v>9.9139316999999998E-3</v>
       </c>
       <c r="AB9">
         <v>1.33563685E-2</v>
@@ -32842,9 +32849,6 @@
       <c r="S10">
         <v>1.400238535E-2</v>
       </c>
-      <c r="T10">
-        <v>4.3119032749999999E-3</v>
-      </c>
       <c r="U10">
         <v>1.0980905075000002E-2</v>
       </c>
@@ -32862,6 +32866,9 @@
       </c>
       <c r="Z10">
         <v>3.1486537000000002E-3</v>
+      </c>
+      <c r="AA10">
+        <v>4.3119032749999999E-3</v>
       </c>
       <c r="AB10">
         <v>2.326937925E-2</v>
@@ -32952,9 +32959,6 @@
       <c r="S11">
         <v>1.3678613400000001E-2</v>
       </c>
-      <c r="T11">
-        <v>6.6943667E-3</v>
-      </c>
       <c r="U11">
         <v>1.0851456750000002E-2</v>
       </c>
@@ -32973,6 +32977,9 @@
       <c r="Z11">
         <v>8.4089272249999996E-3</v>
       </c>
+      <c r="AA11">
+        <v>6.6943667E-3</v>
+      </c>
       <c r="AC11">
         <v>1.4444940500000001E-2</v>
       </c>
@@ -33008,6 +33015,31 @@
       </c>
       <c r="AN11">
         <v>1.9163611500000004E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E09BD3F-D87C-8A40-ABBC-AB728A4E57CC}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1615</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1616</v>
       </c>
     </row>
   </sheetData>

</xml_diff>